<commit_message>
31 st dataes work information
</commit_message>
<xml_diff>
--- a/WRITE4u-work dates-27.xlsx
+++ b/WRITE4u-work dates-27.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="464">
   <si>
     <t>ID:AH20142</t>
   </si>
@@ -1271,9 +1271,6 @@
     <t xml:space="preserve">EXTEND DATE </t>
   </si>
   <si>
-    <t xml:space="preserve">Auto CNN Creditcard frud Dection  </t>
-  </si>
-  <si>
     <t xml:space="preserve">26th </t>
   </si>
   <si>
@@ -1359,13 +1356,73 @@
   </si>
   <si>
     <t>ID:AH21547</t>
+  </si>
+  <si>
+    <t>AH21565</t>
+  </si>
+  <si>
+    <t>29-07-022</t>
+  </si>
+  <si>
+    <t>oracle</t>
+  </si>
+  <si>
+    <t>DS1083</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Analytics + python </t>
+  </si>
+  <si>
+    <t>AH21582</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data analytics </t>
+  </si>
+  <si>
+    <t>29th 4 data set</t>
+  </si>
+  <si>
+    <t>21-07-02022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">start not saying exact data </t>
+  </si>
+  <si>
+    <t xml:space="preserve">w &amp; I </t>
+  </si>
+  <si>
+    <t xml:space="preserve">29-07-2022 writing part </t>
+  </si>
+  <si>
+    <t>Discuse Indranil sir</t>
+  </si>
+  <si>
+    <t>ID:AH21594</t>
+  </si>
+  <si>
+    <t>Client Done</t>
+  </si>
+  <si>
+    <t>AH21596</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no language </t>
+  </si>
+  <si>
+    <t>Data set file  attached 30-07-2022</t>
+  </si>
+  <si>
+    <t>ID:AH21590</t>
+  </si>
+  <si>
+    <t>Exam foramt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1417,13 +1474,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -1436,12 +1486,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF202124"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -1449,12 +1493,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF222222"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -1483,7 +1521,7 @@
       <name val="Roboto"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1515,12 +1553,6 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1540,7 +1572,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1548,9 +1580,8 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1570,62 +1601,44 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="5" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="10" fillId="6" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="5" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="7" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="7" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1634,8 +1647,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="8">
-    <cellStyle name="20% - Accent3" xfId="7" builtinId="38"/>
+  <cellStyles count="7">
     <cellStyle name="Accent2" xfId="2" builtinId="33"/>
     <cellStyle name="Accent5" xfId="1" builtinId="45"/>
     <cellStyle name="Bad" xfId="4" builtinId="27"/>
@@ -1934,10 +1946,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W217"/>
+  <dimension ref="A1:W223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A208" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C222" sqref="C222"/>
+    <sheetView tabSelected="1" topLeftCell="A216" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C223" sqref="C223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
@@ -3783,15 +3795,19 @@
       <c r="C104" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="D104" s="10"/>
+      <c r="D104" s="10" t="s">
+        <v>453</v>
+      </c>
       <c r="E104" s="10" t="s">
-        <v>7</v>
+        <v>454</v>
       </c>
       <c r="F104" s="10"/>
       <c r="G104" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="H104" s="10"/>
+      <c r="H104" s="10" t="s">
+        <v>455</v>
+      </c>
     </row>
     <row r="105" spans="1:8">
       <c r="A105" s="10" t="s">
@@ -4338,27 +4354,27 @@
       <c r="H136" s="10"/>
     </row>
     <row r="137" spans="1:11">
-      <c r="A137" s="11" t="s">
+      <c r="A137" t="s">
         <v>264</v>
       </c>
-      <c r="B137" s="12">
+      <c r="B137">
         <v>44746</v>
       </c>
-      <c r="C137" s="11" t="s">
+      <c r="C137" t="s">
         <v>304</v>
       </c>
-      <c r="D137" s="11" t="s">
+      <c r="D137" t="s">
         <v>266</v>
       </c>
-      <c r="E137" s="11" t="s">
+      <c r="E137" t="s">
         <v>7</v>
       </c>
-      <c r="F137" s="11"/>
-      <c r="G137" s="11" t="s">
+      <c r="F137"/>
+      <c r="G137" t="s">
         <v>265</v>
       </c>
-      <c r="H137" s="11"/>
-      <c r="I137" s="6"/>
+      <c r="H137"/>
+      <c r="I137"/>
       <c r="K137" s="2">
         <v>44756</v>
       </c>
@@ -5035,7 +5051,7 @@
       <c r="H170" s="10"/>
     </row>
     <row r="171" spans="1:8">
-      <c r="A171" s="21" t="s">
+      <c r="A171" s="17" t="s">
         <v>347</v>
       </c>
       <c r="B171" s="9">
@@ -5053,7 +5069,7 @@
       <c r="H171" s="10"/>
     </row>
     <row r="172" spans="1:8">
-      <c r="A172" s="21" t="s">
+      <c r="A172" s="17" t="s">
         <v>350</v>
       </c>
       <c r="B172" s="9">
@@ -5087,13 +5103,13 @@
       <c r="H173" s="10"/>
     </row>
     <row r="174" spans="1:8">
-      <c r="A174" s="21" t="s">
+      <c r="A174" s="17" t="s">
         <v>356</v>
       </c>
       <c r="B174" s="9">
         <v>44756</v>
       </c>
-      <c r="C174" s="22" t="s">
+      <c r="C174" s="18" t="s">
         <v>355</v>
       </c>
       <c r="D174" s="10" t="s">
@@ -5199,7 +5215,7 @@
       <c r="B180" s="9">
         <v>44759</v>
       </c>
-      <c r="C180" s="22" t="s">
+      <c r="C180" s="18" t="s">
         <v>368</v>
       </c>
       <c r="D180" s="10" t="s">
@@ -5211,39 +5227,39 @@
       <c r="H180" s="10"/>
     </row>
     <row r="181" spans="1:13">
-      <c r="A181" s="14" t="s">
+      <c r="A181" s="12" t="s">
         <v>369</v>
       </c>
-      <c r="B181" s="13">
+      <c r="B181" s="11">
         <v>44760</v>
       </c>
-      <c r="C181" s="14" t="s">
+      <c r="C181" s="12" t="s">
         <v>400</v>
       </c>
-      <c r="D181" s="14" t="s">
+      <c r="D181" s="12" t="s">
         <v>401</v>
       </c>
-      <c r="E181" s="14"/>
-      <c r="F181" s="14" t="s">
+      <c r="E181" s="12"/>
+      <c r="F181" s="12" t="s">
         <v>409</v>
       </c>
-      <c r="G181" s="14"/>
+      <c r="G181" s="12"/>
       <c r="H181" s="10"/>
     </row>
     <row r="182" spans="1:13">
-      <c r="A182" s="15" t="s">
+      <c r="A182" t="s">
         <v>193</v>
       </c>
-      <c r="B182" s="16">
+      <c r="B182">
         <v>44760</v>
       </c>
-      <c r="C182" s="15" t="s">
+      <c r="C182" t="s">
         <v>370</v>
       </c>
-      <c r="D182" s="15" t="s">
+      <c r="D182" t="s">
         <v>316</v>
       </c>
-      <c r="E182" s="10"/>
+      <c r="E182"/>
       <c r="F182" s="10"/>
       <c r="G182" s="10"/>
       <c r="H182" s="10"/>
@@ -5264,7 +5280,7 @@
       <c r="E183" s="10" t="s">
         <v>373</v>
       </c>
-      <c r="F183" s="22" t="s">
+      <c r="F183" s="18" t="s">
         <v>374</v>
       </c>
       <c r="G183" s="10" t="s">
@@ -5289,31 +5305,31 @@
       <c r="H184" s="10"/>
     </row>
     <row r="185" spans="1:13" s="5" customFormat="1" ht="14.5">
-      <c r="A185" s="18" t="s">
+      <c r="A185" s="14" t="s">
         <v>377</v>
       </c>
-      <c r="B185" s="17">
+      <c r="B185" s="13">
         <v>44760</v>
       </c>
-      <c r="C185" s="18" t="s">
+      <c r="C185" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D185" s="18" t="s">
+      <c r="D185" s="14" t="s">
         <v>372</v>
       </c>
-      <c r="E185" s="18"/>
-      <c r="F185" s="17">
+      <c r="E185" s="14"/>
+      <c r="F185" s="13">
         <v>44769</v>
       </c>
-      <c r="G185" s="18" t="s">
+      <c r="G185" s="14" t="s">
         <v>389</v>
       </c>
-      <c r="H185" s="18"/>
+      <c r="H185" s="14"/>
       <c r="K185" s="5" t="s">
         <v>414</v>
       </c>
       <c r="M185" s="5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="186" spans="1:13">
@@ -5349,24 +5365,26 @@
       <c r="H187" s="10"/>
     </row>
     <row r="188" spans="1:13" s="6" customFormat="1" ht="14.5">
-      <c r="A188" s="11" t="s">
+      <c r="A188" t="s">
         <v>381</v>
       </c>
-      <c r="B188" s="12">
+      <c r="B188">
         <v>44762</v>
       </c>
-      <c r="C188" s="11" t="s">
+      <c r="C188" t="s">
         <v>382</v>
       </c>
-      <c r="D188" s="11" t="s">
+      <c r="D188" t="s">
         <v>316</v>
       </c>
-      <c r="E188" s="11" t="s">
+      <c r="E188" t="s">
         <v>383</v>
       </c>
-      <c r="F188" s="11"/>
-      <c r="G188" s="11"/>
-      <c r="H188" s="11"/>
+      <c r="F188"/>
+      <c r="G188" t="s">
+        <v>461</v>
+      </c>
+      <c r="H188"/>
     </row>
     <row r="189" spans="1:13">
       <c r="A189" s="10" t="s">
@@ -5401,24 +5419,24 @@
       <c r="H190" s="10"/>
     </row>
     <row r="191" spans="1:13">
-      <c r="A191" s="11" t="s">
+      <c r="A191" t="s">
         <v>387</v>
       </c>
-      <c r="B191" s="12">
+      <c r="B191">
         <v>44761</v>
       </c>
-      <c r="C191" s="11" t="s">
+      <c r="C191" t="s">
         <v>388</v>
       </c>
-      <c r="D191" s="11" t="s">
+      <c r="D191" t="s">
         <v>316</v>
       </c>
-      <c r="E191" s="11" t="s">
+      <c r="E191" t="s">
         <v>383</v>
       </c>
-      <c r="F191" s="11"/>
-      <c r="G191" s="11"/>
-      <c r="H191" s="10"/>
+      <c r="F191"/>
+      <c r="G191"/>
+      <c r="H191"/>
     </row>
     <row r="192" spans="1:13">
       <c r="A192" s="10" t="s">
@@ -5438,7 +5456,7 @@
       <c r="G192" s="10"/>
       <c r="H192" s="10"/>
     </row>
-    <row r="193" spans="1:8">
+    <row r="193" spans="1:9">
       <c r="A193" s="10" t="s">
         <v>392</v>
       </c>
@@ -5456,47 +5474,52 @@
       <c r="G193" s="10"/>
       <c r="H193" s="10"/>
     </row>
-    <row r="194" spans="1:8" ht="16" thickBot="1">
-      <c r="A194" s="19" t="s">
+    <row r="194" spans="1:9" ht="16" thickBot="1">
+      <c r="A194" s="15" t="s">
         <v>394</v>
       </c>
-      <c r="B194" s="20">
+      <c r="B194" s="16">
         <v>44763</v>
       </c>
-      <c r="C194" s="19" t="s">
+      <c r="C194" s="15" t="s">
         <v>317</v>
       </c>
-      <c r="D194" s="19" t="s">
+      <c r="D194" s="15" t="s">
         <v>289</v>
       </c>
-      <c r="E194" s="19" t="s">
+      <c r="E194" s="15" t="s">
         <v>395</v>
       </c>
       <c r="F194" s="10"/>
       <c r="G194" s="10"/>
       <c r="H194" s="10"/>
     </row>
-    <row r="195" spans="1:8" ht="16" thickTop="1">
-      <c r="A195" s="23" t="s">
+    <row r="195" spans="1:9" ht="16" thickTop="1">
+      <c r="A195" t="s">
         <v>396</v>
       </c>
-      <c r="B195" s="24">
-        <v>44763</v>
-      </c>
-      <c r="C195" s="23" t="s">
+      <c r="B195" t="s">
+        <v>452</v>
+      </c>
+      <c r="C195" t="s">
         <v>13</v>
       </c>
-      <c r="D195" s="23" t="s">
+      <c r="D195" t="s">
+        <v>411</v>
+      </c>
+      <c r="E195" s="10" t="s">
+        <v>352</v>
+      </c>
+      <c r="F195" t="s">
         <v>415</v>
       </c>
-      <c r="E195" s="23"/>
-      <c r="F195" s="23" t="s">
-        <v>416</v>
-      </c>
-      <c r="G195" s="10"/>
-      <c r="H195" s="10"/>
-    </row>
-    <row r="196" spans="1:8">
+      <c r="G195" t="s">
+        <v>451</v>
+      </c>
+      <c r="H195"/>
+      <c r="I195"/>
+    </row>
+    <row r="196" spans="1:9">
       <c r="A196" s="10" t="s">
         <v>397</v>
       </c>
@@ -5512,7 +5535,7 @@
       <c r="G196" s="10"/>
       <c r="H196" s="10"/>
     </row>
-    <row r="197" spans="1:8">
+    <row r="197" spans="1:9">
       <c r="A197" s="10" t="s">
         <v>398</v>
       </c>
@@ -5528,7 +5551,7 @@
       <c r="G197" s="10"/>
       <c r="H197" s="10"/>
     </row>
-    <row r="198" spans="1:8">
+    <row r="198" spans="1:9">
       <c r="A198" s="10" t="s">
         <v>399</v>
       </c>
@@ -5544,7 +5567,7 @@
       <c r="G198" s="10"/>
       <c r="H198" s="10"/>
     </row>
-    <row r="199" spans="1:8">
+    <row r="199" spans="1:9">
       <c r="A199" s="10" t="s">
         <v>402</v>
       </c>
@@ -5564,7 +5587,7 @@
       <c r="G199" s="10"/>
       <c r="H199" s="10"/>
     </row>
-    <row r="200" spans="1:8">
+    <row r="200" spans="1:9">
       <c r="A200" s="10" t="s">
         <v>390</v>
       </c>
@@ -5582,7 +5605,7 @@
       <c r="G200" s="10"/>
       <c r="H200" s="10"/>
     </row>
-    <row r="201" spans="1:8">
+    <row r="201" spans="1:9">
       <c r="A201" s="10" t="s">
         <v>402</v>
       </c>
@@ -5602,7 +5625,7 @@
       <c r="G201" s="10"/>
       <c r="H201" s="10"/>
     </row>
-    <row r="202" spans="1:8">
+    <row r="202" spans="1:9">
       <c r="A202" s="10" t="s">
         <v>408</v>
       </c>
@@ -5622,7 +5645,7 @@
       <c r="G202" s="10"/>
       <c r="H202" s="10"/>
     </row>
-    <row r="203" spans="1:8">
+    <row r="203" spans="1:9">
       <c r="A203" s="10" t="s">
         <v>410</v>
       </c>
@@ -5642,7 +5665,7 @@
       <c r="G203" s="10"/>
       <c r="H203" s="10"/>
     </row>
-    <row r="204" spans="1:8">
+    <row r="204" spans="1:9">
       <c r="A204" s="10" t="s">
         <v>396</v>
       </c>
@@ -5662,54 +5685,54 @@
       <c r="G204" s="10"/>
       <c r="H204" s="10"/>
     </row>
-    <row r="205" spans="1:8">
+    <row r="205" spans="1:9">
       <c r="A205" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B205" s="2">
         <v>44766</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D205" s="1" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="206" spans="1:8">
+    <row r="206" spans="1:9">
       <c r="A206" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B206" s="2">
         <v>44767</v>
       </c>
-      <c r="C206" s="25" t="s">
+      <c r="C206" s="19" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9">
+      <c r="A207" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="B207" s="1" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="207" spans="1:8">
-      <c r="A207" s="1" t="s">
+      <c r="C207" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="D207" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="B207" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="C207" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="D207" s="1" t="s">
+      <c r="E207" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="E207" s="1" t="s">
+      <c r="F207" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="F207" s="1" t="s">
+    </row>
+    <row r="208" spans="1:9">
+      <c r="A208" s="1" t="s">
         <v>427</v>
-      </c>
-    </row>
-    <row r="208" spans="1:8">
-      <c r="A208" s="1" t="s">
-        <v>428</v>
       </c>
       <c r="B208" s="2">
         <v>44737</v>
@@ -5723,13 +5746,13 @@
     </row>
     <row r="209" spans="1:6">
       <c r="A209" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B209" s="2">
         <v>44768</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D209" s="1" t="s">
         <v>289</v>
@@ -5737,38 +5760,38 @@
     </row>
     <row r="210" spans="1:6">
       <c r="A210" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B210" s="2">
         <v>44768</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D210" s="1" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="211" spans="1:6">
-      <c r="A211" s="26" t="s">
-        <v>433</v>
+      <c r="A211" s="20" t="s">
+        <v>432</v>
       </c>
       <c r="B211" s="2">
         <v>44800</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="212" spans="1:6">
       <c r="A212" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B212" s="2">
         <v>44801</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D212" s="1" t="s">
         <v>289</v>
@@ -5776,71 +5799,152 @@
     </row>
     <row r="213" spans="1:6">
       <c r="A213" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B213" s="2">
         <v>44770</v>
       </c>
       <c r="C213" s="1" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6">
+      <c r="A214" s="21" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="214" spans="1:6">
-      <c r="A214" s="27" t="s">
+      <c r="B214" s="22">
+        <v>44770</v>
+      </c>
+      <c r="C214" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D214" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="E214" s="22">
+        <v>44804</v>
+      </c>
+      <c r="F214" s="21"/>
+    </row>
+    <row r="215" spans="1:6">
+      <c r="A215" s="23" t="s">
         <v>439</v>
       </c>
-      <c r="B214" s="28">
+      <c r="B215" s="22">
         <v>44770</v>
       </c>
-      <c r="C214" s="27" t="s">
+      <c r="C215" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D214" s="27" t="s">
-        <v>289</v>
-      </c>
-      <c r="E214" s="28">
+      <c r="D215" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="E215" s="22">
         <v>44804</v>
       </c>
-      <c r="F214" s="27"/>
-    </row>
-    <row r="215" spans="1:6">
-      <c r="A215" s="29" t="s">
-        <v>440</v>
-      </c>
-      <c r="B215" s="28">
-        <v>44770</v>
-      </c>
-      <c r="C215" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="D215" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="E215" s="28">
-        <v>44804</v>
-      </c>
-      <c r="F215" s="27"/>
+      <c r="F215" s="21"/>
     </row>
     <row r="216" spans="1:6">
       <c r="A216" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B216" s="2">
         <v>44770</v>
       </c>
       <c r="C216" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="D216" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="D216" s="1" t="s">
+    </row>
+    <row r="217" spans="1:6">
+      <c r="A217" s="20" t="s">
         <v>443</v>
-      </c>
-    </row>
-    <row r="217" spans="1:6">
-      <c r="A217" s="26" t="s">
-        <v>444</v>
       </c>
       <c r="B217" s="2">
         <v>44770</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6">
+      <c r="A218" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C218" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="D218" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6">
+      <c r="A219" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="B219" s="2">
+        <v>44771</v>
+      </c>
+      <c r="C219" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="D219" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E219" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6">
+      <c r="A220" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="B220" s="2">
+        <v>44771</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D220" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6">
+      <c r="A221" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="B221" s="2">
+        <v>44772</v>
+      </c>
+      <c r="D221" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E221" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6">
+      <c r="A222" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="B222" s="2">
+        <v>44772</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6">
+      <c r="A223" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="B223" s="2">
+        <v>44772</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>463</v>
       </c>
     </row>
   </sheetData>

</xml_diff>